<commit_message>
Some manual tests added
</commit_message>
<xml_diff>
--- a/data/SeleniumProject.xlsx
+++ b/data/SeleniumProject.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elite\eclipse-workspace\FinalProject\SeleniumProject\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{162963CF-9BEE-4709-A489-8053A8C0B294}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2466A1D7-4227-42B4-B8C7-E5D5222ACD9A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="logInCorrect" sheetId="1" r:id="rId1"/>
-    <sheet name="invalidUsername" sheetId="2" r:id="rId2"/>
-    <sheet name="invalidPassword" sheetId="4" r:id="rId3"/>
-    <sheet name="noCredentials" sheetId="3" r:id="rId4"/>
+    <sheet name="Test scenarios" sheetId="5" r:id="rId1"/>
+    <sheet name="Login form" sheetId="1" r:id="rId2"/>
+    <sheet name="Address" sheetId="2" r:id="rId3"/>
+    <sheet name="My information" sheetId="4" r:id="rId4"/>
+    <sheet name="My wishlist" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="120">
   <si>
     <t>Preconditions</t>
   </si>
@@ -162,12 +163,317 @@
   <si>
     <t>#4</t>
   </si>
+  <si>
+    <r>
+      <t>Login form functionality at</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> http://automationpractice.com/</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Login form functionality at </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>http://automationpractice.com/</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">User address tests at </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>http://automationpractice.com/</t>
+    </r>
+  </si>
+  <si>
+    <t>Add a user's address</t>
+  </si>
+  <si>
+    <t>Update a user's address</t>
+  </si>
+  <si>
+    <t>Remove a user's address</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Wishlist tests at </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>http://automationpractice.com/</t>
+    </r>
+  </si>
+  <si>
+    <t>Create a wishlist</t>
+  </si>
+  <si>
+    <t>Add multiple wishlists</t>
+  </si>
+  <si>
+    <t>Remove a wishlist</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Log in with an invalid email</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Log in with an invalid password</t>
+  </si>
+  <si>
+    <t>User is logged in and "My Account" section displayed</t>
+  </si>
+  <si>
+    <t>The window reloads and "My addresses" section is displayed, with all the user's addresses displayed, details visible.</t>
+  </si>
+  <si>
+    <t>Click on the "Update" button</t>
+  </si>
+  <si>
+    <t>The window reloads and the details of the selected address are displayed.</t>
+  </si>
+  <si>
+    <t>Kornelija Stankovića</t>
+  </si>
+  <si>
+    <t>Address is entered and visible and the input field background turns green</t>
+  </si>
+  <si>
+    <t>Delete the previous address and enter a new one, like "Kornelija Stankovića"</t>
+  </si>
+  <si>
+    <t>In the field marked "Address (Line 2)", enter "11"</t>
+  </si>
+  <si>
+    <t>Click on "My addresses"</t>
+  </si>
+  <si>
+    <t>Click on the "Add a new address" button</t>
+  </si>
+  <si>
+    <t>The window reloads and a form is displayed with a number of inputs for a new address, first name and last name already filled in</t>
+  </si>
+  <si>
+    <t>Address line 2 entered and visible in the field, input field background now green</t>
+  </si>
+  <si>
+    <t>Enter a street name in the "Address" field</t>
+  </si>
+  <si>
+    <t>Enter a street number in the "Address (Line 2)" field</t>
+  </si>
+  <si>
+    <t>Click on the "Update" button again</t>
+  </si>
+  <si>
+    <t>Acacia Avenue</t>
+  </si>
+  <si>
+    <t>Delete the test address and enter the original one, like "Acacia Avenue"</t>
+  </si>
+  <si>
+    <t>In the field marked "Address (Line 2)", enter "22"</t>
+  </si>
+  <si>
+    <t>Click on the "Save" button</t>
+  </si>
+  <si>
+    <t>The window reloads and the user is returned to "My Address" section, details changed are clearly visible in the address field.</t>
+  </si>
+  <si>
+    <t>Enter a city in the "City" field</t>
+  </si>
+  <si>
+    <t>Hackney</t>
+  </si>
+  <si>
+    <t>Arizona</t>
+  </si>
+  <si>
+    <t>Test adresa</t>
+  </si>
+  <si>
+    <t>City is entered and visible and the input field background turns green</t>
+  </si>
+  <si>
+    <t>Choose a state from the dropdown field labeled "State"</t>
+  </si>
+  <si>
+    <t>State is visibly chosen in the dropdown menu</t>
+  </si>
+  <si>
+    <t>Type in a ZIP code in the field labeled "Zip/Postal Code"</t>
+  </si>
+  <si>
+    <t>Postal code is entered and visible and the input field background turns green</t>
+  </si>
+  <si>
+    <t>+3846892569</t>
+  </si>
+  <si>
+    <t>+3689541666</t>
+  </si>
+  <si>
+    <t>In the field "Home phone" type in a phone number</t>
+  </si>
+  <si>
+    <t>In the field "Mobile phone" type in a phone number</t>
+  </si>
+  <si>
+    <t>Home phone is entered and visible and the input field background turns green</t>
+  </si>
+  <si>
+    <t>Mobile phone number is entered and visible and the input field background turns green</t>
+  </si>
+  <si>
+    <t>In a field labeled "Please assign an address title for future reference. *", type in the name/alias of the address</t>
+  </si>
+  <si>
+    <t>Alias is entered and visible and the input field background turns green</t>
+  </si>
+  <si>
+    <t>Click the "Save" button</t>
+  </si>
+  <si>
+    <t>User is now taken to "My Addresses" overview, with all addresses entered by the user visible</t>
+  </si>
+  <si>
+    <t>click on the "Delete" button of the other address</t>
+  </si>
+  <si>
+    <t>Press "OK"</t>
+  </si>
+  <si>
+    <t>A confirmation prompt pops up and asks the user to confirm the deletion of the address - "Are you sure?"</t>
+  </si>
+  <si>
+    <t>The second address is now deleted with only one address remaining in the "My addresses" section</t>
+  </si>
+  <si>
+    <t>Edit personal information</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Edit user's personal information at </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>http://automationpractice.com/</t>
+    </r>
+  </si>
+  <si>
+    <t>Click on "My personal information"</t>
+  </si>
+  <si>
+    <t>The window reloads and  "My personal information" section is displayed, with all the personal information input forms visible.</t>
+  </si>
+  <si>
+    <t>In the field "Name", enter a name</t>
+  </si>
+  <si>
+    <t>Mladen</t>
+  </si>
+  <si>
+    <t>Original address now displayed in the address field, the background of the input field now light green.</t>
+  </si>
+  <si>
+    <t>User's name now displayed in the address field, the background of the input field now light green.</t>
+  </si>
+  <si>
+    <t>User's last name now displayed in the address field, the background of the input field now light green.</t>
+  </si>
+  <si>
+    <t>In the field "Last name", enter a name</t>
+  </si>
+  <si>
+    <t>Tomic</t>
+  </si>
+  <si>
+    <t>In the field "E-mail address" enter an email</t>
+  </si>
+  <si>
+    <t>User's email now displayed in the address field, the background of the input field light green.</t>
+  </si>
+  <si>
+    <t>Choose a day from the dropdown menu</t>
+  </si>
+  <si>
+    <t>Choose a month from the dropdown menu</t>
+  </si>
+  <si>
+    <t>Choose a year from the dropdown menu</t>
+  </si>
+  <si>
+    <t>November</t>
+  </si>
+  <si>
+    <t>In the "Current Password" field, enter the current password of the user</t>
+  </si>
+  <si>
+    <t>The password now entered and visible as dots in the form input.</t>
+  </si>
+  <si>
+    <t>Year now displayed and visible in the input of the dropdown form.</t>
+  </si>
+  <si>
+    <t>Month now displayed and visible in the input of the dropdown form.</t>
+  </si>
+  <si>
+    <t>Day now displayed and visible in the input of the dropdown form.</t>
+  </si>
+  <si>
+    <t>Press the "Save" button</t>
+  </si>
+  <si>
+    <t>The window reloads and a notification is displayed confirming that personal information has been changed</t>
+  </si>
+  <si>
+    <t>Your personal information has been successfully updated.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -205,6 +511,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -233,7 +546,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -254,11 +567,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -541,26 +872,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC1F9645-37F8-4476-B01C-F2FC47829A1F}">
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.44140625" customWidth="1"/>
-    <col min="2" max="2" width="6" customWidth="1"/>
-    <col min="3" max="3" width="28.6640625" customWidth="1"/>
-    <col min="4" max="4" width="21" customWidth="1"/>
-    <col min="5" max="5" width="27.33203125" customWidth="1"/>
-    <col min="6" max="6" width="22.5546875" customWidth="1"/>
-    <col min="7" max="7" width="44.77734375" customWidth="1"/>
-    <col min="8" max="8" width="12.77734375" customWidth="1"/>
+    <col min="1" max="1" width="29.33203125" customWidth="1"/>
+    <col min="2" max="2" width="5.33203125" customWidth="1"/>
+    <col min="3" max="3" width="37.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -570,81 +896,112 @@
       <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
-        <v>9</v>
+    </row>
+    <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E3" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="E4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="E5" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6" t="s">
-        <v>24</v>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B4" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B5" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B6" s="6"/>
+      <c r="C6" s="10"/>
+    </row>
+    <row r="7" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C8" s="11"/>
+    </row>
+    <row r="9" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B10" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B11" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B14" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B15" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -654,11 +1011,309 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H22"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="28.21875" customWidth="1"/>
+    <col min="2" max="2" width="5.33203125" customWidth="1"/>
+    <col min="3" max="3" width="26.88671875" customWidth="1"/>
+    <col min="4" max="4" width="15.88671875" customWidth="1"/>
+    <col min="5" max="5" width="38.77734375" customWidth="1"/>
+    <col min="6" max="6" width="24.6640625" customWidth="1"/>
+    <col min="7" max="7" width="48.77734375" customWidth="1"/>
+    <col min="8" max="8" width="12.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="6"/>
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="6"/>
+      <c r="G6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F7" s="6"/>
+    </row>
+    <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E9" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="6"/>
+      <c r="G9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E11" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F13" s="6"/>
+    </row>
+    <row r="14" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E15" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="6"/>
+      <c r="G15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="E16" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E17" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E18" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E21" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="E22" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F10" r:id="rId1" xr:uid="{D2902766-4FD4-4426-8DDC-F966DB712C63}"/>
+    <hyperlink ref="F16" r:id="rId2" xr:uid="{ACD1F158-6792-42B2-9070-2AB41B3A4E00}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0E5C442-71B0-42B8-B82C-4D0F1AEB26F0}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -666,7 +1321,7 @@
     <col min="1" max="1" width="28.21875" customWidth="1"/>
     <col min="2" max="2" width="5.33203125" customWidth="1"/>
     <col min="3" max="3" width="25.33203125" customWidth="1"/>
-    <col min="4" max="4" width="15.88671875" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
     <col min="5" max="5" width="38.77734375" customWidth="1"/>
     <col min="6" max="6" width="23" customWidth="1"/>
     <col min="7" max="7" width="48.77734375" customWidth="1"/>
@@ -700,93 +1355,288 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
-        <v>9</v>
+      <c r="A2" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E3" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" t="s">
-        <v>15</v>
+        <v>6</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="5"/>
+      <c r="G2" s="12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E3" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>18</v>
+        <v>58</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>56</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>19</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E5" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G5" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" s="13">
+        <v>11</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E6" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F6" s="13"/>
+      <c r="G6" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E7" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="F7" s="6"/>
+      <c r="G7" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E8" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E9" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F9" s="6">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="E6" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>29</v>
+      <c r="G9" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="E10" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F10" s="13"/>
+      <c r="G10" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="F12" s="5"/>
+      <c r="G12" s="12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="E13" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E14" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E15" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F15" s="13">
+        <v>11</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E16" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E17" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E18" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F18" s="6">
+        <v>15000</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E19" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E20" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="E21" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E22" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="F24" s="5"/>
+      <c r="G24" s="12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E25" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E26" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="F4" r:id="rId1" xr:uid="{7E778207-50E7-40D8-B03E-0D43663710BD}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9E207AC-4FF3-4B31-85BE-3B84DF83AE62}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.21875" customWidth="1"/>
+    <col min="1" max="1" width="32.109375" customWidth="1"/>
     <col min="2" max="2" width="5.33203125" customWidth="1"/>
-    <col min="3" max="3" width="25.33203125" customWidth="1"/>
+    <col min="3" max="3" width="22.44140625" customWidth="1"/>
     <col min="4" max="4" width="15.88671875" customWidth="1"/>
     <col min="5" max="5" width="38.77734375" customWidth="1"/>
-    <col min="6" max="6" width="23" customWidth="1"/>
+    <col min="6" max="6" width="40.5546875" customWidth="1"/>
     <col min="7" max="7" width="48.77734375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -813,84 +1663,126 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
-        <v>9</v>
+    <row r="2" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>96</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E3" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="E4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>19</v>
+        <v>6</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="F2" s="5"/>
+      <c r="G2" s="12" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E3" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E4" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="E5" s="3" t="s">
-        <v>27</v>
+        <v>106</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" t="s">
-        <v>22</v>
+        <v>18</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="E6" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" t="s">
-        <v>30</v>
+        <v>108</v>
+      </c>
+      <c r="F6" s="6">
+        <v>20</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>29</v>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E7" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E8" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="F8" s="6">
+        <v>1984</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E9" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E10" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="F4" r:id="rId1" xr:uid="{313078A9-591E-4AD2-A8D1-42C648B8BD3D}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CE0C6BE-737D-4693-B8EB-2F42E1B413A4}">
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A2" sqref="A2:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -962,7 +1854,7 @@
       <c r="E4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="8" t="s">
         <v>33</v>
       </c>
       <c r="G4" s="2" t="s">

</xml_diff>